<commit_message>
Client from Client-Server is Done
</commit_message>
<xml_diff>
--- a/Операции.xlsx
+++ b/Операции.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>Код операции</t>
   </si>
@@ -139,6 +139,45 @@
   </si>
   <si>
     <t>Картинка</t>
+  </si>
+  <si>
+    <t>Выдать действующие этажи</t>
+  </si>
+  <si>
+    <t>Выдать все этажи</t>
+  </si>
+  <si>
+    <t>Номера и названия этажей</t>
+  </si>
+  <si>
+    <t>Загрузить схему</t>
+  </si>
+  <si>
+    <t>Выдать id следующей точки</t>
+  </si>
+  <si>
+    <t>Выдать id следующего Этажа</t>
+  </si>
+  <si>
+    <t>Создать менеджера</t>
+  </si>
+  <si>
+    <t>Загрузить список всех менеджеров</t>
+  </si>
+  <si>
+    <t>Схема</t>
+  </si>
+  <si>
+    <t>логины всех менеджеров</t>
+  </si>
+  <si>
+    <t>Свободный номер точки</t>
+  </si>
+  <si>
+    <t>Свободный номер этажа</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -481,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,13 +794,102 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1">
+        <v>19</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Server in Client-Server is done
</commit_message>
<xml_diff>
--- a/Операции.xlsx
+++ b/Операции.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>Код операции</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Добавить этаж к действующим</t>
+  </si>
+  <si>
+    <t>Убрать из действующих</t>
+  </si>
+  <si>
+    <t>Удалить менеджера</t>
+  </si>
+  <si>
+    <t>Сменить пароль</t>
+  </si>
+  <si>
+    <t>login pass</t>
   </si>
 </sst>
 </file>
@@ -520,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,6 +904,56 @@
       </c>
       <c r="D27" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1">
+        <v>25</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="1">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1">
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
connect to DataBase & Floor, Space, Exhibit , Autorization is done
</commit_message>
<xml_diff>
--- a/Операции.xlsx
+++ b/Операции.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Код операции</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Удалить схему этажа</t>
   </si>
   <si>
-    <t>* Добавить этаж к текущей схеме</t>
-  </si>
-  <si>
-    <t>*Удалить</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -193,6 +187,9 @@
   </si>
   <si>
     <t>login pass</t>
+  </si>
+  <si>
+    <t>ВЫЧЕРКНУТО</t>
   </si>
 </sst>
 </file>
@@ -209,12 +206,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -229,11 +232,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -535,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,6 +555,7 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -577,12 +586,12 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -591,12 +600,12 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -610,16 +619,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,7 +771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -776,188 +785,180 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1">
-        <v>16</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="1">
-        <v>17</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B23" s="1">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="1">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="1">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="1">
-        <v>20</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="1">
-        <v>21</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
       <c r="B26" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
       <c r="B29" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" s="1">
-        <v>26</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="1">
-        <v>27</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>